<commit_message>
add new page object for Add new customer
</commit_message>
<xml_diff>
--- a/TestData/LoginData.xlsx
+++ b/TestData/LoginData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ngocchien/PycharmProjects/Selenium/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E60AA0E8-0E13-864F-8FD5-4325159A92C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFB44567-6A28-384C-A5A1-7B01E3BCE9F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="43900" yWindow="-3580" windowWidth="28040" windowHeight="17260" xr2:uid="{5EEE7633-2804-364A-8977-09ACAD4E1437}"/>
   </bookViews>
@@ -47,29 +47,29 @@
     <t>exp</t>
   </si>
   <si>
-    <t>buingocchien5596</t>
-  </si>
-  <si>
-    <t>traikimnguu5596</t>
-  </si>
-  <si>
     <t>Pass</t>
   </si>
   <si>
-    <t>buingocchien55961</t>
-  </si>
-  <si>
-    <t>traikimnguu55961</t>
-  </si>
-  <si>
     <t>Fail</t>
+  </si>
+  <si>
+    <t>admin@yourstore.com</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>admin1@yourstore.com</t>
+  </si>
+  <si>
+    <t>admin1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -81,6 +81,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -124,15 +132,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -448,7 +459,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -469,50 +480,56 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
+      <c r="A4" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
+      <c r="A5" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{5F6185E0-7FA2-9F46-BAA9-8B42706CAA07}"/>
+    <hyperlink ref="A3:A5" r:id="rId2" display="admin@yourstore.com" xr:uid="{D2A6F44B-6262-9B47-AB5F-25C642C31668}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{798663C9-6D26-C142-915A-E55F9BC42081}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{B65197C7-4B9F-D549-BF85-3358D7C13569}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>